<commit_message>
Tests adjusted to new changes in initial DB for tests
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTests/manifestUploadTemplateTest2.xlsx
+++ b/src/test/resources/excelTests/manifestUploadTemplateTest2.xlsx
@@ -1881,7 +1881,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="53" t="n">
-        <v>43900.0</v>
+        <v>43901.0</v>
       </c>
       <c r="C3" s="64" t="n">
         <v>0.4375</v>
@@ -1893,7 +1893,7 @@
         <v>114</v>
       </c>
       <c r="F3" s="43" t="n">
-        <v>43901.0</v>
+        <v>43902.0</v>
       </c>
       <c r="G3" s="45" t="n">
         <v>0.6458333333333334</v>
@@ -1909,7 +1909,7 @@
         <v>113</v>
       </c>
       <c r="N3" s="49" t="n">
-        <v>43904.0</v>
+        <v>43905.0</v>
       </c>
       <c r="O3" s="55" t="n">
         <v>0.4583333333333333</v>
@@ -1921,7 +1921,7 @@
         <v>138</v>
       </c>
       <c r="R3" s="50" t="n">
-        <v>43910.0</v>
+        <v>43911.0</v>
       </c>
       <c r="S3" s="75" t="n">
         <v>0.4166666666666667</v>

</xml_diff>